<commit_message>
[#PAB-428] add postcodes and itl regions to the data model
</commit_message>
<xml_diff>
--- a/tests/controller_tests/resources/Data_Model_v3.7_EXAMPLE.xlsx
+++ b/tests/controller_tests/resources/Data_Model_v3.7_EXAMPLE.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SnapeN\Dev\funding-service-design-post-award-data-store\tests\controller_tests\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DobbsC\PycharmProjects\funding-service-design-post-award-data-store\tests\controller_tests\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68AB6C83-C326-434A-8D25-E6C7CF2361E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{298987C2-895A-443C-8482-7114591D781A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5175" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="7" xr2:uid="{00652EC3-4B88-41F9-B7C9-30F3C6E2549B}"/>
+    <workbookView xWindow="2190" yWindow="1800" windowWidth="32310" windowHeight="15435" firstSheet="6" activeTab="6" xr2:uid="{00652EC3-4B88-41F9-B7C9-30F3C6E2549B}"/>
   </bookViews>
   <sheets>
     <sheet name="Submission_Ref" sheetId="20" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1923" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1932" uniqueCount="406">
   <si>
     <t>Submission ID</t>
   </si>
@@ -1260,6 +1260,15 @@
   </si>
   <si>
     <t>GIS Provided</t>
+  </si>
+  <si>
+    <t>Postcodes</t>
+  </si>
+  <si>
+    <t>SW1A 2AA, example location</t>
+  </si>
+  <si>
+    <t>SW1A 2AA,BT1 1AA</t>
   </si>
 </sst>
 </file>
@@ -1413,6 +1422,18 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
@@ -1427,18 +1448,6 @@
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1474,7 +1483,7 @@
     <tableColumn id="3" xr3:uid="{8950D16B-3257-4FD9-9209-91782FB1847C}" name="Townsfund Funding"/>
     <tableColumn id="4" xr3:uid="{42D9447C-F1D5-4248-8FD8-D6A1E53CD4FA}" name="Private Sector Funding Required"/>
     <tableColumn id="5" xr3:uid="{D2CCA7A1-0565-4275-8174-63583B5641B3}" name="Private Sector Funding Secured"/>
-    <tableColumn id="1" xr3:uid="{839BF95B-13D1-4C30-A711-1F8084FA3A46}" name="Additional Comments" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{839BF95B-13D1-4C30-A711-1F8084FA3A46}" name="Additional Comments" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1525,12 +1534,12 @@
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{8537E16F-E797-4E37-88C9-434B275E47FF}" name="Project ID"/>
     <tableColumn id="9" xr3:uid="{D4160626-660D-43E1-8026-277F46FD67C0}" name="Programme ID"/>
-    <tableColumn id="2" xr3:uid="{570DDDB8-B36A-46F5-92BC-965A389460F7}" name="Start_Date" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{C6CD430A-E931-4BB6-BB6E-DDB49D07DF48}" name="End_Date" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{570DDDB8-B36A-46F5-92BC-965A389460F7}" name="Start_Date" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{C6CD430A-E931-4BB6-BB6E-DDB49D07DF48}" name="End_Date" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{900E6096-72C0-4BB1-83C2-947FF46110E9}" name="Outcome"/>
     <tableColumn id="5" xr3:uid="{79C9218D-BBE0-4D8F-A799-35A0ECCBA6EA}" name="UnitofMeasurement"/>
     <tableColumn id="6" xr3:uid="{FF2CB41E-3A92-492C-AE6D-D96513330D69}" name="GeographyIndicator"/>
-    <tableColumn id="7" xr3:uid="{7B14AE8F-255A-468D-9664-209C5422934F}" name="Amount" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{7B14AE8F-255A-468D-9664-209C5422934F}" name="Amount" dataDxfId="0"/>
     <tableColumn id="8" xr3:uid="{0F2A7BA4-AEDC-42D9-94CD-5CD8E178E408}" name="Actual/Forecast"/>
     <tableColumn id="11" xr3:uid="{421424EF-099E-4EAA-9115-B2CFFB224759}" name="Higher Frequency"/>
   </tableColumns>
@@ -1616,9 +1625,9 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{58B2215B-BB35-4202-BB72-BEDFDCA878F6}" name="Table12" displayName="Table12" ref="A1:I9" totalsRowShown="0">
-  <autoFilter ref="A1:I9" xr:uid="{58B2215B-BB35-4202-BB72-BEDFDCA878F6}"/>
-  <tableColumns count="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{58B2215B-BB35-4202-BB72-BEDFDCA878F6}" name="Table12" displayName="Table12" ref="A1:J9" totalsRowShown="0">
+  <autoFilter ref="A1:J9" xr:uid="{58B2215B-BB35-4202-BB72-BEDFDCA878F6}"/>
+  <tableColumns count="10">
     <tableColumn id="3" xr3:uid="{839B46E7-B168-4B9E-A694-7DCDD22CB60B}" name="Project ID"/>
     <tableColumn id="7" xr3:uid="{7A79B4CF-CCAB-447B-B607-9620980DD5FE}" name="Submission ID"/>
     <tableColumn id="2" xr3:uid="{677D3277-CB52-4DE9-9DED-741A1FC4FD2E}" name="Programme ID"/>
@@ -1626,6 +1635,7 @@
     <tableColumn id="4" xr3:uid="{7F49D6D7-6D62-463F-AEAA-F506EF803F0C}" name="Primary Intervention Theme"/>
     <tableColumn id="5" xr3:uid="{D8406B66-B5E0-47A0-B8AC-9236F3A24B8D}" name="Single or Multiple Locations"/>
     <tableColumn id="1" xr3:uid="{106938F4-FA9F-4D44-95FC-F6EA7DB8029A}" name="Locations"/>
+    <tableColumn id="11" xr3:uid="{003140ED-B03C-4E83-820F-290EA7E88C46}" name="Postcodes"/>
     <tableColumn id="8" xr3:uid="{71285834-179B-4577-8EA8-5D36A100ED48}" name="GIS Provided"/>
     <tableColumn id="9" xr3:uid="{CCEBE39A-8B8B-47CB-8B79-166126BA6E9A}" name="Lat/Long"/>
   </tableColumns>
@@ -1663,8 +1673,8 @@
     <tableColumn id="2" xr3:uid="{4446533C-3A7E-4CC9-A147-F8E4F6E140A5}" name="Funding Source Name"/>
     <tableColumn id="3" xr3:uid="{B77FCEE0-D5EB-4D8D-B8EE-81B086635306}" name="Funding Source Type"/>
     <tableColumn id="4" xr3:uid="{09EFF7B4-5759-483D-8894-DA967909D34C}" name="Secured"/>
-    <tableColumn id="1" xr3:uid="{F0E11478-A8DE-4C32-891D-004E7C1CC338}" name="Start_Date" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{D171D8BE-5473-4026-9113-F75851A24BA3}" name="End_Date" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{F0E11478-A8DE-4C32-891D-004E7C1CC338}" name="Start_Date" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{D171D8BE-5473-4026-9113-F75851A24BA3}" name="End_Date" dataDxfId="4"/>
     <tableColumn id="8" xr3:uid="{EBBED273-C141-4990-8ACA-C4CDB99F78FC}" name="Spend for Reporting Period"/>
     <tableColumn id="10" xr3:uid="{5927EFE4-3ED3-46F2-9BA7-6ABE2C41AE29}" name="Actual / Forecast"/>
   </tableColumns>
@@ -9708,10 +9718,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{230DDC13-8AF0-4935-A621-88AD3C9E9DD9}">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9720,12 +9730,13 @@
     <col min="2" max="4" width="21.28515625" customWidth="1"/>
     <col min="5" max="5" width="36.85546875" customWidth="1"/>
     <col min="6" max="6" width="23.42578125" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -9748,13 +9759,16 @@
         <v>26</v>
       </c>
       <c r="H1" t="s">
+        <v>403</v>
+      </c>
+      <c r="I1" t="s">
         <v>402</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -9774,16 +9788,19 @@
         <v>28</v>
       </c>
       <c r="G2" t="s">
+        <v>404</v>
+      </c>
+      <c r="H2" t="s">
         <v>29</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>87</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -9806,10 +9823,13 @@
         <v>29</v>
       </c>
       <c r="H3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -9832,13 +9852,16 @@
         <v>35</v>
       </c>
       <c r="H4" t="s">
+        <v>405</v>
+      </c>
+      <c r="I4" t="s">
         <v>98</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -9861,10 +9884,13 @@
         <v>29</v>
       </c>
       <c r="H5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -9886,11 +9912,14 @@
       <c r="G6" t="s">
         <v>29</v>
       </c>
-      <c r="I6" t="s">
+      <c r="H6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -9912,8 +9941,11 @@
       <c r="G7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>41</v>
       </c>
@@ -9936,13 +9968,16 @@
         <v>29</v>
       </c>
       <c r="H8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" t="s">
         <v>87</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -9965,14 +10000,17 @@
         <v>29</v>
       </c>
       <c r="H9" t="s">
+        <v>29</v>
+      </c>
+      <c r="I9" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
@@ -10041,8 +10079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8E8DE40-009E-4B3E-BD8A-08B04A259F7E}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10709,26 +10747,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="681fe441-c46c-4ea5-a5c5-b45872725697">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="83a87e31-bf32-46ab-8e70-9fa18461fa4d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AB5DDB95A7ECBD49AA08D06BA3EF1CDA" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="95a99fb7649f76cf16eb4f5cafa7cbc2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="681fe441-c46c-4ea5-a5c5-b45872725697" xmlns:ns3="6bac55d2-c587-47e2-866b-bbb6fe14d104" xmlns:ns4="83a87e31-bf32-46ab-8e70-9fa18461fa4d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cbf7ff0d2c127a9a42e650b92ffbc482" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="681fe441-c46c-4ea5-a5c5-b45872725697"/>
@@ -10970,26 +10988,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70073AC4-B26C-493C-8C25-29DBD67F7B7B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="681fe441-c46c-4ea5-a5c5-b45872725697"/>
-    <ds:schemaRef ds:uri="83a87e31-bf32-46ab-8e70-9fa18461fa4d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CA70E21-41D5-415B-B329-A133B7922149}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="681fe441-c46c-4ea5-a5c5-b45872725697">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="83a87e31-bf32-46ab-8e70-9fa18461fa4d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9931E176-D5AF-4D57-88FA-0E21DE56657D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11009,6 +11028,25 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CA70E21-41D5-415B-B329-A133B7922149}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70073AC4-B26C-493C-8C25-29DBD67F7B7B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="681fe441-c46c-4ea5-a5c5-b45872725697"/>
+    <ds:schemaRef ds:uri="83a87e31-bf32-46ab-8e70-9fa18461fa4d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{95c71a0f-75e1-4c8f-90e2-641c9351dd98}" enabled="1" method="Standard" siteId="{3e0088dc-0629-4ae6-aa8c-813e7a296f50}" removed="0"/>

</xml_diff>

<commit_message>
[BAU] fix date serialization
</commit_message>
<xml_diff>
--- a/tests/controller_tests/resources/Data_Model_v3.7_EXAMPLE.xlsx
+++ b/tests/controller_tests/resources/Data_Model_v3.7_EXAMPLE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DobbsC\PycharmProjects\funding-service-design-post-award-data-store\tests\controller_tests\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{298987C2-895A-443C-8482-7114591D781A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B293F42-C7AC-43FC-9F02-4AB8C432C2D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2190" yWindow="1800" windowWidth="32310" windowHeight="15435" firstSheet="6" activeTab="6" xr2:uid="{00652EC3-4B88-41F9-B7C9-30F3C6E2549B}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" firstSheet="7" activeTab="7" xr2:uid="{00652EC3-4B88-41F9-B7C9-30F3C6E2549B}"/>
   </bookViews>
   <sheets>
     <sheet name="Submission_Ref" sheetId="20" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1932" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1934" uniqueCount="408">
   <si>
     <t>Submission ID</t>
   </si>
@@ -1269,6 +1269,12 @@
   </si>
   <si>
     <t>SW1A 2AA,BT1 1AA</t>
+  </si>
+  <si>
+    <t>12/13/14</t>
+  </si>
+  <si>
+    <t>12/13/16</t>
   </si>
 </sst>
 </file>
@@ -2919,7 +2925,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3423617-CC86-44FD-A69A-E6E9F4D332E6}">
   <dimension ref="A1:I120"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:D15"/>
     </sheetView>
   </sheetViews>
@@ -6658,7 +6664,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4717C6AB-1205-4862-A377-00B1F94B35FD}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
@@ -9720,8 +9726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{230DDC13-8AF0-4935-A621-88AD3C9E9DD9}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10079,8 +10085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8E8DE40-009E-4B3E-BD8A-08B04A259F7E}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10164,6 +10170,9 @@
       <c r="I2">
         <v>3</v>
       </c>
+      <c r="L2" s="1" t="s">
+        <v>406</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -10193,6 +10202,7 @@
       <c r="I3">
         <v>3</v>
       </c>
+      <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -10222,14 +10232,19 @@
       <c r="I4">
         <v>5</v>
       </c>
+      <c r="L4" s="1" t="s">
+        <v>407</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
+      <c r="L5" s="1"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
+      <c r="L6" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -10248,7 +10263,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFBE28E4-3DB0-487F-AAD0-E345678244B7}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
[FIX] outcome categories endpoint shouldn't return none types
</commit_message>
<xml_diff>
--- a/tests/controller_tests/resources/Data_Model_v3.7_EXAMPLE.xlsx
+++ b/tests/controller_tests/resources/Data_Model_v3.7_EXAMPLE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DobbsC\PycharmProjects\funding-service-design-post-award-data-store\tests\controller_tests\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F3C8067-9751-4DF3-B3FD-577599EE77C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{782A93F3-5EB5-4692-807C-5D6FB2B2AFF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="75" yWindow="1605" windowWidth="21600" windowHeight="11385" firstSheet="7" activeTab="8" xr2:uid="{00652EC3-4B88-41F9-B7C9-30F3C6E2549B}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="38700" windowHeight="15435" firstSheet="7" activeTab="13" xr2:uid="{00652EC3-4B88-41F9-B7C9-30F3C6E2549B}"/>
   </bookViews>
   <sheets>
     <sheet name="Submission_Ref" sheetId="20" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1671" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1672" uniqueCount="406">
   <si>
     <t>Programme ID</t>
   </si>
@@ -1266,6 +1266,9 @@
   </si>
   <si>
     <t>12/13/16</t>
+  </si>
+  <si>
+    <t>Example Null Category Outcome</t>
   </si>
 </sst>
 </file>
@@ -1513,8 +1516,8 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{16381EAE-E4C5-4567-95AA-33EE9251DC1D}" name="Table6" displayName="Table6" ref="A1:B65" totalsRowShown="0">
-  <autoFilter ref="A1:B65" xr:uid="{16381EAE-E4C5-4567-95AA-33EE9251DC1D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{16381EAE-E4C5-4567-95AA-33EE9251DC1D}" name="Table6" displayName="Table6" ref="A1:B66" totalsRowShown="0">
+  <autoFilter ref="A1:B66" xr:uid="{16381EAE-E4C5-4567-95AA-33EE9251DC1D}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{9DA3BB6A-A48F-4CC5-AF90-C29356A04C9A}" name="Outcome_Name"/>
     <tableColumn id="2" xr3:uid="{5DD9E4B4-A6A7-4E19-ACD9-7418586D71E4}" name="Outcome_Category"/>
@@ -5678,10 +5681,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4566479-493F-467C-B8F7-F354284ED4E4}">
-  <dimension ref="A1:B65"/>
+  <dimension ref="A1:B66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6208,6 +6211,11 @@
       </c>
       <c r="B65" t="s">
         <v>229</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>405</v>
       </c>
     </row>
   </sheetData>
@@ -6223,7 +6231,7 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9438,7 +9446,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFBE28E4-3DB0-487F-AAD0-E345678244B7}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -9891,26 +9899,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="681fe441-c46c-4ea5-a5c5-b45872725697">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="83a87e31-bf32-46ab-8e70-9fa18461fa4d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AB5DDB95A7ECBD49AA08D06BA3EF1CDA" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="95a99fb7649f76cf16eb4f5cafa7cbc2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="681fe441-c46c-4ea5-a5c5-b45872725697" xmlns:ns3="6bac55d2-c587-47e2-866b-bbb6fe14d104" xmlns:ns4="83a87e31-bf32-46ab-8e70-9fa18461fa4d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cbf7ff0d2c127a9a42e650b92ffbc482" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="681fe441-c46c-4ea5-a5c5-b45872725697"/>
@@ -10152,26 +10140,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70073AC4-B26C-493C-8C25-29DBD67F7B7B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="681fe441-c46c-4ea5-a5c5-b45872725697"/>
-    <ds:schemaRef ds:uri="83a87e31-bf32-46ab-8e70-9fa18461fa4d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CA70E21-41D5-415B-B329-A133B7922149}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="681fe441-c46c-4ea5-a5c5-b45872725697">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="83a87e31-bf32-46ab-8e70-9fa18461fa4d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9931E176-D5AF-4D57-88FA-0E21DE56657D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10191,6 +10180,25 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CA70E21-41D5-415B-B329-A133B7922149}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70073AC4-B26C-493C-8C25-29DBD67F7B7B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="681fe441-c46c-4ea5-a5c5-b45872725697"/>
+    <ds:schemaRef ds:uri="83a87e31-bf32-46ab-8e70-9fa18461fa4d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{95c71a0f-75e1-4c8f-90e2-641c9351dd98}" enabled="1" method="Standard" siteId="{3e0088dc-0629-4ae6-aa8c-813e7a296f50}" removed="0"/>

</xml_diff>